<commit_message>
added my list of acceptance tests and edited one of my user stories
</commit_message>
<xml_diff>
--- a/User Stories [TEMPLATE].xlsx
+++ b/User Stories [TEMPLATE].xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t xml:space="preserve"> EPIC</t>
   </si>
@@ -172,6 +172,15 @@
   </si>
   <si>
     <t>As a registered user, I want to browse all fields.</t>
+  </si>
+  <si>
+    <t>Verify that the user can view all experts of one of the available list of fields. Verify that the returned results are complete and correct.</t>
+  </si>
+  <si>
+    <t>As a registered user, I want to be able to do an basic search.</t>
+  </si>
+  <si>
+    <t>Verify that the user can search by expert name and  that the returned results are complete and correct.</t>
   </si>
 </sst>
 </file>
@@ -994,7 +1003,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1290,14 +1299,16 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:19" ht="45">
       <c r="A6" s="9"/>
       <c r="B6" s="10" t="s">
         <v>48</v>
       </c>
       <c r="C6" s="11"/>
       <c r="D6" s="12"/>
-      <c r="E6" s="13"/>
+      <c r="E6" s="13" t="s">
+        <v>49</v>
+      </c>
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
       <c r="H6" s="14"/>
@@ -1340,14 +1351,16 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:19" ht="33.75">
       <c r="A7" s="9"/>
       <c r="B7" s="10" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="12"/>
-      <c r="E7" s="13"/>
+      <c r="E7" s="13" t="s">
+        <v>51</v>
+      </c>
       <c r="F7" s="13"/>
       <c r="G7" s="13"/>
       <c r="H7" s="14"/>

</xml_diff>